<commit_message>
Update template cashflow to fix report cashflow
</commit_message>
<xml_diff>
--- a/enhancement/final_cashflow.xlsx
+++ b/enhancement/final_cashflow.xlsx
@@ -80,31 +80,31 @@
     <t>Deva</t>
   </si>
   <si>
+    <t>Rangga R</t>
+  </si>
+  <si>
+    <t>Rangga A</t>
+  </si>
+  <si>
+    <t>Marc</t>
+  </si>
+  <si>
+    <t>Kipo</t>
+  </si>
+  <si>
+    <t>Ferdian</t>
+  </si>
+  <si>
+    <t>Debora</t>
+  </si>
+  <si>
+    <t>Sri Zonihastuty</t>
+  </si>
+  <si>
+    <t>Total Masuk:</t>
+  </si>
+  <si>
     <t>Total Keluar:</t>
-  </si>
-  <si>
-    <t>Rangga R</t>
-  </si>
-  <si>
-    <t>Rangga A</t>
-  </si>
-  <si>
-    <t>Marc</t>
-  </si>
-  <si>
-    <t>Kipo</t>
-  </si>
-  <si>
-    <t>Ferdian</t>
-  </si>
-  <si>
-    <t>Debora</t>
-  </si>
-  <si>
-    <t>Sri Zonihastuty</t>
-  </si>
-  <si>
-    <t>Total Masuk:</t>
   </si>
   <si>
     <t>Jumat, 14 November 2025     NBC Padel - Centro Bintaro</t>
@@ -193,7 +193,7 @@
     <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="180" formatCode="[$Rp-421]\ #,##0;[Red]\-[$Rp-421]\ #,##0"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,13 +259,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF0EA5E9"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -766,152 +759,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -931,9 +924,6 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -943,9 +933,6 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -955,39 +942,29 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="180" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="180" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="180" fontId="8" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="180" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -996,7 +973,6 @@
     <xf numFmtId="180" fontId="5" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1389,8 +1365,8 @@
   <sheetPr/>
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H57" sqref="H57"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -1421,7 +1397,7 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-      <c r="K1" s="35"/>
+      <c r="K1" s="26"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
@@ -1436,7 +1412,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="36"/>
+      <c r="K2" s="27"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="3" t="s">
@@ -1453,153 +1429,148 @@
       <c r="H3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="37"/>
-      <c r="J3" s="38" t="s">
+      <c r="I3" s="28"/>
+      <c r="J3" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="38"/>
+      <c r="K3" s="29"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="39"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="39"/>
+      <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="15">
-        <v>75000</v>
-      </c>
-      <c r="C6" s="16">
-        <v>1</v>
-      </c>
-      <c r="D6" s="15">
+      <c r="B6" s="13">
+        <v>75000</v>
+      </c>
+      <c r="C6" s="14">
+        <v>1</v>
+      </c>
+      <c r="D6" s="13">
         <v>75000</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="13">
         <v>800000</v>
       </c>
-      <c r="I6" s="16">
-        <v>1</v>
-      </c>
-      <c r="J6" s="15">
+      <c r="I6" s="14">
+        <v>1</v>
+      </c>
+      <c r="J6" s="13">
         <v>800000</v>
       </c>
-      <c r="K6" s="39"/>
+      <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="15">
-        <v>75000</v>
-      </c>
-      <c r="C7" s="16">
-        <v>1</v>
-      </c>
-      <c r="D7" s="15">
+      <c r="B7" s="13">
+        <v>75000</v>
+      </c>
+      <c r="C7" s="14">
+        <v>1</v>
+      </c>
+      <c r="D7" s="13">
         <v>75000</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="13">
         <v>55000</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7" s="14">
         <v>3</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="13">
         <v>165000</v>
       </c>
-      <c r="K7" s="39"/>
+      <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="15">
-        <v>75000</v>
-      </c>
-      <c r="C8" s="16">
-        <v>1</v>
-      </c>
-      <c r="D8" s="15">
+      <c r="B8" s="13">
+        <v>75000</v>
+      </c>
+      <c r="C8" s="14">
+        <v>1</v>
+      </c>
+      <c r="D8" s="13">
         <v>75000</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="12"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="40">
-        <f>SUM(J6:J7)</f>
-        <v>965000</v>
-      </c>
-      <c r="K8" s="39"/>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="15">
-        <v>75000</v>
-      </c>
-      <c r="C9" s="16">
-        <v>1</v>
-      </c>
-      <c r="D9" s="15">
+      <c r="B9" s="13">
+        <v>75000</v>
+      </c>
+      <c r="C9" s="14">
+        <v>1</v>
+      </c>
+      <c r="D9" s="13">
         <v>75000</v>
       </c>
       <c r="E9" s="5"/>
@@ -1608,19 +1579,19 @@
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="39"/>
+      <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="15">
-        <v>75000</v>
-      </c>
-      <c r="C10" s="16">
-        <v>1</v>
-      </c>
-      <c r="D10" s="15">
+      <c r="A10" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="13">
+        <v>75000</v>
+      </c>
+      <c r="C10" s="14">
+        <v>1</v>
+      </c>
+      <c r="D10" s="13">
         <v>75000</v>
       </c>
       <c r="E10" s="5"/>
@@ -1629,19 +1600,19 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="39"/>
+      <c r="K10" s="5"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="15">
-        <v>75000</v>
-      </c>
-      <c r="C11" s="16">
-        <v>1</v>
-      </c>
-      <c r="D11" s="15">
+      <c r="A11" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="13">
+        <v>75000</v>
+      </c>
+      <c r="C11" s="14">
+        <v>1</v>
+      </c>
+      <c r="D11" s="13">
         <v>75000</v>
       </c>
       <c r="E11" s="5"/>
@@ -1650,19 +1621,19 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="39"/>
+      <c r="K11" s="5"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="15">
-        <v>75000</v>
-      </c>
-      <c r="C12" s="16">
-        <v>1</v>
-      </c>
-      <c r="D12" s="15">
+      <c r="A12" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="13">
+        <v>75000</v>
+      </c>
+      <c r="C12" s="14">
+        <v>1</v>
+      </c>
+      <c r="D12" s="13">
         <v>75000</v>
       </c>
       <c r="E12" s="5"/>
@@ -1671,19 +1642,19 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="39"/>
+      <c r="K12" s="5"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="15">
-        <v>75000</v>
-      </c>
-      <c r="C13" s="16">
-        <v>1</v>
-      </c>
-      <c r="D13" s="15">
+      <c r="A13" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="13">
+        <v>75000</v>
+      </c>
+      <c r="C13" s="14">
+        <v>1</v>
+      </c>
+      <c r="D13" s="13">
         <v>75000</v>
       </c>
       <c r="E13" s="5"/>
@@ -1692,19 +1663,19 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="39"/>
+      <c r="K13" s="5"/>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="15">
-        <v>75000</v>
-      </c>
-      <c r="C14" s="16">
-        <v>1</v>
-      </c>
-      <c r="D14" s="15">
+      <c r="A14" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="13">
+        <v>75000</v>
+      </c>
+      <c r="C14" s="14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="13">
         <v>75000</v>
       </c>
       <c r="E14" s="5"/>
@@ -1713,19 +1684,19 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="39"/>
+      <c r="K14" s="5"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="15">
-        <v>75000</v>
-      </c>
-      <c r="C15" s="16">
-        <v>1</v>
-      </c>
-      <c r="D15" s="15">
+      <c r="A15" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="13">
+        <v>75000</v>
+      </c>
+      <c r="C15" s="14">
+        <v>1</v>
+      </c>
+      <c r="D15" s="13">
         <v>75000</v>
       </c>
       <c r="E15" s="5"/>
@@ -1734,38 +1705,43 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
-      <c r="K15" s="39"/>
+      <c r="K15" s="5"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="21">
+      <c r="A16" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="16">
         <f>SUM(D6:D15)</f>
         <v>750000</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="39"/>
+      <c r="G16" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="30">
+        <f>SUM(J14:J15)</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="41"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="31"/>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="3" t="s">
@@ -1782,153 +1758,144 @@
       <c r="H18" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I18" s="37"/>
-      <c r="J18" s="38" t="s">
+      <c r="I18" s="28"/>
+      <c r="J18" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="K18" s="38"/>
+      <c r="K18" s="29"/>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="39"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="5"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="H20" s="12" t="s">
+      <c r="H20" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I20" s="12" t="s">
+      <c r="I20" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J20" s="12" t="s">
+      <c r="J20" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="K20" s="39"/>
+      <c r="K20" s="5"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="15">
-        <v>75000</v>
-      </c>
-      <c r="C21" s="16">
-        <v>1</v>
-      </c>
-      <c r="D21" s="15">
+      <c r="B21" s="13">
+        <v>75000</v>
+      </c>
+      <c r="C21" s="14">
+        <v>1</v>
+      </c>
+      <c r="D21" s="13">
         <v>75000</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
-      <c r="G21" s="17" t="s">
+      <c r="G21" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="H21" s="15">
+      <c r="H21" s="13">
         <v>800000</v>
       </c>
-      <c r="I21" s="16">
-        <v>1</v>
-      </c>
-      <c r="J21" s="15">
+      <c r="I21" s="14">
+        <v>1</v>
+      </c>
+      <c r="J21" s="13">
         <v>800000</v>
       </c>
-      <c r="K21" s="39"/>
+      <c r="K21" s="5"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="15">
-        <v>75000</v>
-      </c>
-      <c r="C22" s="16">
-        <v>1</v>
-      </c>
-      <c r="D22" s="15">
+      <c r="B22" s="13">
+        <v>75000</v>
+      </c>
+      <c r="C22" s="14">
+        <v>1</v>
+      </c>
+      <c r="D22" s="13">
         <v>75000</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="17" t="s">
+      <c r="G22" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="H22" s="15">
+      <c r="H22" s="13">
         <v>55000</v>
       </c>
-      <c r="I22" s="16">
+      <c r="I22" s="14">
         <v>3</v>
       </c>
-      <c r="J22" s="15">
+      <c r="J22" s="13">
         <v>165000</v>
       </c>
-      <c r="K22" s="39"/>
+      <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="15">
-        <v>75000</v>
-      </c>
-      <c r="C23" s="16">
-        <v>1</v>
-      </c>
-      <c r="D23" s="15">
+      <c r="B23" s="13">
+        <v>75000</v>
+      </c>
+      <c r="C23" s="14">
+        <v>1</v>
+      </c>
+      <c r="D23" s="13">
         <v>75000</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="40">
-        <f>SUM(J21:J22)</f>
-        <v>965000</v>
-      </c>
-      <c r="K23" s="39"/>
+      <c r="K23" s="5"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="15">
-        <v>75000</v>
-      </c>
-      <c r="C24" s="16">
-        <v>1</v>
-      </c>
-      <c r="D24" s="15">
+      <c r="B24" s="13">
+        <v>75000</v>
+      </c>
+      <c r="C24" s="14">
+        <v>1</v>
+      </c>
+      <c r="D24" s="13">
         <v>75000</v>
       </c>
       <c r="E24" s="5"/>
@@ -1937,19 +1904,19 @@
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
-      <c r="K24" s="39"/>
+      <c r="K24" s="5"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="15">
-        <v>75000</v>
-      </c>
-      <c r="C25" s="16">
-        <v>1</v>
-      </c>
-      <c r="D25" s="15">
+      <c r="B25" s="13">
+        <v>75000</v>
+      </c>
+      <c r="C25" s="14">
+        <v>1</v>
+      </c>
+      <c r="D25" s="13">
         <v>75000</v>
       </c>
       <c r="E25" s="5"/>
@@ -1958,19 +1925,19 @@
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
-      <c r="K25" s="39"/>
+      <c r="K25" s="5"/>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="15">
-        <v>75000</v>
-      </c>
-      <c r="C26" s="16">
-        <v>1</v>
-      </c>
-      <c r="D26" s="15">
+      <c r="B26" s="13">
+        <v>75000</v>
+      </c>
+      <c r="C26" s="14">
+        <v>1</v>
+      </c>
+      <c r="D26" s="13">
         <v>75000</v>
       </c>
       <c r="E26" s="5"/>
@@ -1979,19 +1946,19 @@
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
-      <c r="K26" s="39"/>
+      <c r="K26" s="5"/>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="15">
-        <v>75000</v>
-      </c>
-      <c r="C27" s="16">
-        <v>1</v>
-      </c>
-      <c r="D27" s="15">
+      <c r="B27" s="13">
+        <v>75000</v>
+      </c>
+      <c r="C27" s="14">
+        <v>1</v>
+      </c>
+      <c r="D27" s="13">
         <v>75000</v>
       </c>
       <c r="E27" s="5"/>
@@ -2000,19 +1967,19 @@
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
-      <c r="K27" s="39"/>
+      <c r="K27" s="5"/>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="15">
-        <v>75000</v>
-      </c>
-      <c r="C28" s="16">
-        <v>1</v>
-      </c>
-      <c r="D28" s="15">
+      <c r="B28" s="13">
+        <v>75000</v>
+      </c>
+      <c r="C28" s="14">
+        <v>1</v>
+      </c>
+      <c r="D28" s="13">
         <v>75000</v>
       </c>
       <c r="E28" s="5"/>
@@ -2021,19 +1988,19 @@
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
-      <c r="K28" s="39"/>
+      <c r="K28" s="5"/>
     </row>
     <row r="29" spans="1:11">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="15">
-        <v>75000</v>
-      </c>
-      <c r="C29" s="16">
-        <v>1</v>
-      </c>
-      <c r="D29" s="15">
+      <c r="B29" s="13">
+        <v>75000</v>
+      </c>
+      <c r="C29" s="14">
+        <v>1</v>
+      </c>
+      <c r="D29" s="13">
         <v>75000</v>
       </c>
       <c r="E29" s="5"/>
@@ -2042,19 +2009,19 @@
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
-      <c r="K29" s="39"/>
+      <c r="K29" s="5"/>
     </row>
     <row r="30" spans="1:11">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="15">
-        <v>75000</v>
-      </c>
-      <c r="C30" s="16">
-        <v>1</v>
-      </c>
-      <c r="D30" s="15">
+      <c r="B30" s="13">
+        <v>75000</v>
+      </c>
+      <c r="C30" s="14">
+        <v>1</v>
+      </c>
+      <c r="D30" s="13">
         <v>75000</v>
       </c>
       <c r="E30" s="5"/>
@@ -2063,37 +2030,42 @@
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
-      <c r="K30" s="39"/>
+      <c r="K30" s="5"/>
     </row>
     <row r="31" spans="1:11">
-      <c r="A31" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="21">
+      <c r="A31" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="16">
         <f>SUM(D21:D30)</f>
         <v>750000</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="39"/>
+      <c r="G31" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="30">
+        <f>SUM(J21:J22)</f>
+        <v>965000</v>
+      </c>
+      <c r="K31" s="5"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="22"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="22"/>
-      <c r="J32" s="22"/>
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="3" t="s">
@@ -2110,8 +2082,8 @@
       <c r="H33" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="I33" s="37"/>
-      <c r="J33" s="42" t="s">
+      <c r="I33" s="28"/>
+      <c r="J33" s="32" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2119,84 +2091,76 @@
       <c r="A34" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
-      <c r="G34" s="10" t="s">
+      <c r="G34" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="10"/>
-      <c r="K34" s="39"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="5"/>
     </row>
     <row r="35" spans="1:11">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
-      <c r="G35" s="13" t="s">
+      <c r="G35" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="H35" s="12" t="s">
+      <c r="H35" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I35" s="12" t="s">
+      <c r="I35" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J35" s="12" t="s">
+      <c r="J35" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="K35" s="39"/>
+      <c r="K35" s="5"/>
     </row>
     <row r="36" spans="1:11">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="15">
-        <v>75000</v>
-      </c>
-      <c r="C36" s="16">
-        <v>1</v>
-      </c>
-      <c r="D36" s="15">
+      <c r="B36" s="13">
+        <v>75000</v>
+      </c>
+      <c r="C36" s="14">
+        <v>1</v>
+      </c>
+      <c r="D36" s="13">
         <v>75000</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
-      <c r="G36" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H36" s="18"/>
-      <c r="I36" s="18"/>
-      <c r="J36" s="40">
-        <v>0</v>
-      </c>
-      <c r="K36" s="39"/>
+      <c r="K36" s="5"/>
     </row>
     <row r="37" spans="1:11">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="15">
-        <v>75000</v>
-      </c>
-      <c r="C37" s="16">
-        <v>1</v>
-      </c>
-      <c r="D37" s="15">
+      <c r="B37" s="13">
+        <v>75000</v>
+      </c>
+      <c r="C37" s="14">
+        <v>1</v>
+      </c>
+      <c r="D37" s="13">
         <v>75000</v>
       </c>
       <c r="E37" s="5"/>
@@ -2205,19 +2169,19 @@
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
-      <c r="K37" s="39"/>
+      <c r="K37" s="5"/>
     </row>
     <row r="38" spans="1:11">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B38" s="15">
-        <v>75000</v>
-      </c>
-      <c r="C38" s="16">
-        <v>1</v>
-      </c>
-      <c r="D38" s="15">
+      <c r="B38" s="13">
+        <v>75000</v>
+      </c>
+      <c r="C38" s="14">
+        <v>1</v>
+      </c>
+      <c r="D38" s="13">
         <v>75000</v>
       </c>
       <c r="E38" s="5"/>
@@ -2226,19 +2190,19 @@
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
-      <c r="K38" s="39"/>
+      <c r="K38" s="5"/>
     </row>
     <row r="39" spans="1:11">
-      <c r="A39" s="14" t="s">
+      <c r="A39" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="15">
-        <v>75000</v>
-      </c>
-      <c r="C39" s="16">
-        <v>1</v>
-      </c>
-      <c r="D39" s="15">
+      <c r="B39" s="13">
+        <v>75000</v>
+      </c>
+      <c r="C39" s="14">
+        <v>1</v>
+      </c>
+      <c r="D39" s="13">
         <v>75000</v>
       </c>
       <c r="E39" s="5"/>
@@ -2247,19 +2211,19 @@
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
-      <c r="K39" s="39"/>
+      <c r="K39" s="5"/>
     </row>
     <row r="40" spans="1:11">
-      <c r="A40" s="14" t="s">
+      <c r="A40" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B40" s="15">
-        <v>75000</v>
-      </c>
-      <c r="C40" s="16">
-        <v>1</v>
-      </c>
-      <c r="D40" s="15">
+      <c r="B40" s="13">
+        <v>75000</v>
+      </c>
+      <c r="C40" s="14">
+        <v>1</v>
+      </c>
+      <c r="D40" s="13">
         <v>75000</v>
       </c>
       <c r="E40" s="5"/>
@@ -2268,19 +2232,19 @@
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
-      <c r="K40" s="39"/>
+      <c r="K40" s="5"/>
     </row>
     <row r="41" spans="1:11">
-      <c r="A41" s="14" t="s">
+      <c r="A41" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B41" s="15">
-        <v>75000</v>
-      </c>
-      <c r="C41" s="16">
-        <v>1</v>
-      </c>
-      <c r="D41" s="15">
+      <c r="B41" s="13">
+        <v>75000</v>
+      </c>
+      <c r="C41" s="14">
+        <v>1</v>
+      </c>
+      <c r="D41" s="13">
         <v>75000</v>
       </c>
       <c r="E41" s="5"/>
@@ -2289,19 +2253,19 @@
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
-      <c r="K41" s="39"/>
+      <c r="K41" s="5"/>
     </row>
     <row r="42" spans="1:11">
-      <c r="A42" s="14" t="s">
+      <c r="A42" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B42" s="15">
-        <v>75000</v>
-      </c>
-      <c r="C42" s="16">
-        <v>1</v>
-      </c>
-      <c r="D42" s="15">
+      <c r="B42" s="13">
+        <v>75000</v>
+      </c>
+      <c r="C42" s="14">
+        <v>1</v>
+      </c>
+      <c r="D42" s="13">
         <v>75000</v>
       </c>
       <c r="E42" s="5"/>
@@ -2310,19 +2274,19 @@
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
-      <c r="K42" s="39"/>
+      <c r="K42" s="5"/>
     </row>
     <row r="43" spans="1:11">
-      <c r="A43" s="14" t="s">
+      <c r="A43" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B43" s="15">
-        <v>75000</v>
-      </c>
-      <c r="C43" s="16">
-        <v>1</v>
-      </c>
-      <c r="D43" s="15">
+      <c r="B43" s="13">
+        <v>75000</v>
+      </c>
+      <c r="C43" s="14">
+        <v>1</v>
+      </c>
+      <c r="D43" s="13">
         <v>75000</v>
       </c>
       <c r="E43" s="5"/>
@@ -2331,19 +2295,19 @@
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
-      <c r="K43" s="39"/>
+      <c r="K43" s="5"/>
     </row>
     <row r="44" spans="1:11">
-      <c r="A44" s="14" t="s">
+      <c r="A44" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B44" s="15">
-        <v>75000</v>
-      </c>
-      <c r="C44" s="16">
-        <v>1</v>
-      </c>
-      <c r="D44" s="15">
+      <c r="B44" s="13">
+        <v>75000</v>
+      </c>
+      <c r="C44" s="14">
+        <v>1</v>
+      </c>
+      <c r="D44" s="13">
         <v>75000</v>
       </c>
       <c r="E44" s="5"/>
@@ -2352,19 +2316,19 @@
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
-      <c r="K44" s="39"/>
+      <c r="K44" s="5"/>
     </row>
     <row r="45" spans="1:11">
-      <c r="A45" s="14" t="s">
+      <c r="A45" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B45" s="15">
-        <v>75000</v>
-      </c>
-      <c r="C45" s="16">
-        <v>1</v>
-      </c>
-      <c r="D45" s="15">
+      <c r="B45" s="13">
+        <v>75000</v>
+      </c>
+      <c r="C45" s="14">
+        <v>1</v>
+      </c>
+      <c r="D45" s="13">
         <v>75000</v>
       </c>
       <c r="E45" s="5"/>
@@ -2373,28 +2337,32 @@
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
-      <c r="K45" s="39"/>
+      <c r="K45" s="5"/>
     </row>
     <row r="46" spans="1:11">
-      <c r="A46" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="21">
+      <c r="A46" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46" s="15"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="16">
         <f>SUM(D36:D45)</f>
         <v>750000</v>
       </c>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="5"/>
-      <c r="J46" s="5"/>
-      <c r="K46" s="39"/>
+      <c r="G46" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
+      <c r="J46" s="30">
+        <v>0</v>
+      </c>
+      <c r="K46" s="5"/>
     </row>
     <row r="47" spans="1:11">
-      <c r="A47" s="23"/>
+      <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
@@ -2404,63 +2372,63 @@
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
-      <c r="K47" s="39"/>
+      <c r="K47" s="5"/>
     </row>
     <row r="48" spans="1:11">
-      <c r="A48" s="24" t="s">
+      <c r="A48" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="26"/>
-      <c r="H48" s="26"/>
-      <c r="I48" s="26"/>
-      <c r="J48" s="26"/>
-      <c r="K48" s="39"/>
+      <c r="B48" s="19"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="20"/>
+      <c r="I48" s="20"/>
+      <c r="J48" s="20"/>
+      <c r="K48" s="5"/>
     </row>
     <row r="49" spans="1:11">
-      <c r="A49" s="27" t="s">
+      <c r="A49" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="28"/>
-      <c r="C49" s="28"/>
-      <c r="D49" s="29">
+      <c r="B49" s="21"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="22">
         <f>SUM(D16,D31,D46)</f>
         <v>2250000</v>
       </c>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="30" t="s">
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="H49" s="30"/>
-      <c r="I49" s="30"/>
-      <c r="J49" s="43">
-        <f>SUM(J8,J23,J36)</f>
-        <v>1930000</v>
-      </c>
-      <c r="K49" s="39"/>
+      <c r="H49" s="23"/>
+      <c r="I49" s="23"/>
+      <c r="J49" s="33">
+        <f>SUM(J8,J31,J46)</f>
+        <v>965000</v>
+      </c>
+      <c r="K49" s="5"/>
     </row>
     <row r="50" spans="1:11">
-      <c r="A50" s="31" t="s">
+      <c r="A50" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="32"/>
-      <c r="C50" s="32"/>
-      <c r="D50" s="33">
+      <c r="B50" s="24"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="25">
         <f>D49-J49</f>
-        <v>320000</v>
-      </c>
-      <c r="E50" s="34"/>
-      <c r="F50" s="34"/>
-      <c r="G50" s="34"/>
-      <c r="H50" s="34"/>
-      <c r="I50" s="34"/>
-      <c r="J50" s="34"/>
-      <c r="K50" s="44"/>
+        <v>1285000</v>
+      </c>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="20"/>
+      <c r="J50" s="20"/>
+      <c r="K50" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="26">
@@ -2470,22 +2438,22 @@
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="G4:J4"/>
-    <mergeCell ref="G8:I8"/>
     <mergeCell ref="A16:C16"/>
+    <mergeCell ref="G16:I16"/>
     <mergeCell ref="A17:J17"/>
     <mergeCell ref="A18:D18"/>
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="G19:J19"/>
-    <mergeCell ref="G23:I23"/>
     <mergeCell ref="A31:C31"/>
+    <mergeCell ref="G31:I31"/>
     <mergeCell ref="A32:J32"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="H33:I33"/>
     <mergeCell ref="A34:D34"/>
     <mergeCell ref="G34:J34"/>
-    <mergeCell ref="G36:I36"/>
     <mergeCell ref="A46:C46"/>
+    <mergeCell ref="G46:I46"/>
     <mergeCell ref="A48:E48"/>
     <mergeCell ref="A49:C49"/>
     <mergeCell ref="G49:I49"/>

</xml_diff>